<commit_message>
Revenue and Expenses Completed.
</commit_message>
<xml_diff>
--- a/exported_member.xlsx
+++ b/exported_member.xlsx
@@ -104,21 +104,21 @@
     <t>9496017942</t>
   </si>
   <si>
+    <t>ജിജിൻ ഫ്രാൻസിസ്</t>
+  </si>
+  <si>
+    <t>jijinfrancisanna@gmail.com</t>
+  </si>
+  <si>
+    <t>amlqaW5mcmFuY2lzYW5uYQ==</t>
+  </si>
+  <si>
+    <t>9846417927</t>
+  </si>
+  <si>
     <t>SUPER_ADMIN</t>
   </si>
   <si>
-    <t>ജിജിൻ ഫ്രാൻസിസ്</t>
-  </si>
-  <si>
-    <t>jijinfrancisanna@gmail.com</t>
-  </si>
-  <si>
-    <t>amlqaW5mcmFuY2lzYW5uYQ==</t>
-  </si>
-  <si>
-    <t>9846417927</t>
-  </si>
-  <si>
     <t>ജീജോ ജേക്കബ്</t>
   </si>
   <si>
@@ -248,7 +248,7 @@
     <t>amF5ZXNoa2s=</t>
   </si>
   <si>
-    <t>MemberModel(no=6, memberName=ലൂയിസ് ജോസഫ്, emailId=luisjoseph6551@gmail.com, password=bHVpc2pvc2VwaDY1NTE=, memberType=PRIMARY, role=USER, referenceMember=null, memberDOB=2025-05-17, mobileNumber=9947886919, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
+    <t>MemberModel(no=6, memberName=ലൂയിസ് ജോസഫ്, emailId=luisjoseph6551@gmail.com, password=bHVpc2pvc2VwaDY1NTE=, memberType=PRIMARY, role=USER, memberDOB=2025-05-17, mobileNumber=9947886919, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
   </si>
   <si>
     <t>SECONDARY</t>
@@ -281,7 +281,7 @@
     <t>dmluZWVzaGNoZWxsYXBwYW4=</t>
   </si>
   <si>
-    <t>MemberModel(no=5, memberName=ജിജോ ജോൺ, emailId=jijojohn777@gmail.com, password=amlqb2pvaG43Nzc=, memberType=PRIMARY, role=SUPER_ADMIN, referenceMember=null, memberDOB=2025-12-20, mobileNumber=9895415828, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
+    <t>MemberModel(no=5, memberName=ജിജോ ജോൺ, emailId=jijojohn777@gmail.com, password=amlqb2pvaG43Nzc=, memberType=PRIMARY, role=SUPER_ADMIN, memberDOB=2025-12-20, mobileNumber=9895415828, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
   </si>
   <si>
     <t>റോയ്  മാത്യൂ</t>
@@ -293,7 +293,7 @@
     <t>cm95bWF0aGV3</t>
   </si>
   <si>
-    <t>MemberModel(no=12, memberName=സുജിത്ത് കൃഷ്ണാ, emailId=sujithskrishna@gmail.com, password=c3VqaXRoc2tyaXNobmE=, memberType=PRIMARY, role=SUPER_ADMIN, referenceMember=null, memberDOB=2025-07-06, mobileNumber=9845375129, address1=Kaithavalappil House, place=Parayakad PO, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688540)</t>
+    <t>MemberModel(no=12, memberName=സുജിത്ത് കൃഷ്ണാ, emailId=sujithskrishna@gmail.com, password=c3VqaXRoc2tyaXNobmE=, memberType=PRIMARY, role=SUPER_ADMIN, memberDOB=2025-07-06, mobileNumber=9845375129, address1=Kaithavalappil House, place=Parayakad PO, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688540)</t>
   </si>
   <si>
     <t>ഷീല ഭാസി</t>
@@ -305,7 +305,7 @@
     <t>c2hlZWxhYmhhc2k=</t>
   </si>
   <si>
-    <t>MemberModel(no=3, memberName=ജിജിൻ ഫ്രാൻസിസ്, emailId=jijinfrancisanna@gmail.com, password=amlqaW5mcmFuY2lzYW5uYQ==, memberType=PRIMARY, role=SUPER_ADMIN, referenceMember=null, memberDOB=2025-11-18, mobileNumber=9846417927, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
+    <t>MemberModel(no=3, memberName=ജിജിൻ ഫ്രാൻസിസ്, emailId=jijinfrancisanna@gmail.com, password=amlqaW5mcmFuY2lzYW5uYQ==, memberType=PRIMARY, role=SUPER_ADMIN, memberDOB=2025-11-18, mobileNumber=9846417927, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
   </si>
   <si>
     <t>സുജാതാ</t>
@@ -317,7 +317,7 @@
     <t>c3VqYXRoYQ==</t>
   </si>
   <si>
-    <t>MemberModel(no=10, memberName=സരിത റഫയൽ, emailId=saritharaphel@gmail.com, password=c2FyaXRoYXJhcGhlbA==, memberType=PRIMARY, role=USER, referenceMember=null, memberDOB=2025-05-16, mobileNumber=7736544685, address1=null, place=null, taluk=Kottayam, district=Kottayam, state=Kerala, pincode=688537)</t>
+    <t>MemberModel(no=10, memberName=സരിത റഫയൽ, emailId=saritharaphel@gmail.com, password=c2FyaXRoYXJhcGhlbA==, memberType=PRIMARY, role=USER, memberDOB=2025-05-16, mobileNumber=7736544685, address1=null, place=null, taluk=Kottayam, district=Kottayam, state=Kerala, pincode=688537)</t>
   </si>
   <si>
     <t>മേരി മൈക്കിൽ</t>
@@ -329,7 +329,7 @@
     <t>bWFycnltaWNoYWVs</t>
   </si>
   <si>
-    <t>MemberModel(no=7, memberName=മനേഷ് മൈക്കിൽ, emailId=manesh.micheal@gmail.com, password=bWFuZXNoLm1pY2hlYWw=, memberType=PRIMARY, role=SUPER_ADMIN, referenceMember=null, memberDOB=2025-11-07, mobileNumber=9995227002, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
+    <t>MemberModel(no=7, memberName=മനേഷ് മൈക്കിൽ, emailId=manesh.micheal@gmail.com, password=bWFuZXNoLm1pY2hlYWw=, memberType=PRIMARY, role=USER, memberDOB=2025-11-07, mobileNumber=9995227002, address1=null, place=null, taluk=Cherthala, district=Alappuzha, state=Kerala, pincode=688537)</t>
   </si>
   <si>
     <t>അച്ചു</t>
@@ -519,7 +519,7 @@
         <v>24</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s" s="0">
         <v>33</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>34</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>45979.0</v>
@@ -562,7 +562,7 @@
         <v>24</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -605,7 +605,7 @@
         <v>24</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -648,7 +648,7 @@
         <v>24</v>
       </c>
       <c r="O6" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -734,7 +734,7 @@
         <v>24</v>
       </c>
       <c r="O8" t="s" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -953,7 +953,7 @@
         <v>24</v>
       </c>
       <c r="O13" t="s" s="0">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">

</xml_diff>